<commit_message>
Retiré la colonne minutes d’ORS
</commit_message>
<xml_diff>
--- a/template2021-2022.xlsx
+++ b/template2021-2022.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t xml:space="preserve">Demande de Crédit Temps Syndical 2021-2022</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve">Heures d'obligations de service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minutes d'obligations de service → saisir 0</t>
   </si>
   <si>
     <t xml:space="preserve">Code Corps (voir annexe)</t>
@@ -478,7 +475,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -726,13 +723,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="13.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.42"/>
@@ -743,6 +740,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -759,7 +757,6 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="17.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="3" t="str">
@@ -1054,7 +1051,6 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="52.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="s">
@@ -1087,14 +1083,10 @@
       <c r="J24" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="K24" s="15" t="s">
+      <c r="K24" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
+      <c r="L24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="18" t="str">
@@ -1107,15 +1099,14 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="21" t="str">
-        <f aca="false">IF(AND(B25="",C25="",D25="",E25="",G25="",I25="",J25=""),"",(IF(OR(B25="",C25="",D25="",E25="",G25="",I25="",J25=""),"Donnée manquante",((E25*60+F25)/(G25*60+H25)))))</f>
-        <v/>
-      </c>
-      <c r="L25" s="22" t="str">
-        <f aca="false">IF(OR(K25="Donnée manquante",K25=""),"",$D$64-SUM($K$25:K25,$C$49))</f>
+      <c r="H25" s="20"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="21" t="str">
+        <f aca="false">IF(AND(B25="",C25="",D25="",E25="",G25="",H25="",I25=""),"",(IF(OR(B25="",C25="",D25="",E25="",G25="",H25="",I25=""),"Donnée manquante",((E25*60+F25)/(G25*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K25" s="22" t="str">
+        <f aca="false">IF(OR(J25="Donnée manquante",J25=""),"",$D$64-SUM($J$25:J25,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1130,15 +1121,14 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="21" t="str">
-        <f aca="false">IF(AND(B26="",C26="",D26="",E26="",G26="",I26="",J26=""),"",(IF(OR(B26="",C26="",D26="",E26="",G26="",I26="",J26=""),"Donnée manquante",((E26*60+F26)/(G26*60+H26)))))</f>
-        <v/>
-      </c>
-      <c r="L26" s="22" t="str">
-        <f aca="false">IF(OR(K26="Donnée manquante",K26=""),"",$D$64-SUM($K$25:K26,$C$49))</f>
+      <c r="H26" s="20"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="21" t="str">
+        <f aca="false">IF(AND(B26="",C26="",D26="",E26="",G26="",H26="",I26=""),"",(IF(OR(B26="",C26="",D26="",E26="",G26="",H26="",I26=""),"Donnée manquante",((E26*60+F26)/(G26*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K26" s="22" t="str">
+        <f aca="false">IF(OR(J26="Donnée manquante",J26=""),"",$D$64-SUM($J$25:J26,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1153,15 +1143,14 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="21" t="str">
-        <f aca="false">IF(AND(B27="",C27="",D27="",E27="",G27="",I27="",J27=""),"",(IF(OR(B27="",C27="",D27="",E27="",G27="",I27="",J27=""),"Donnée manquante",((E27*60+F27)/(G27*60+H27)))))</f>
-        <v/>
-      </c>
-      <c r="L27" s="22" t="str">
-        <f aca="false">IF(OR(K27="Donnée manquante",K27=""),"",$D$64-SUM($K$25:K27,$C$49))</f>
+      <c r="H27" s="20"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="21" t="str">
+        <f aca="false">IF(AND(B27="",C27="",D27="",E27="",G27="",H27="",I27=""),"",(IF(OR(B27="",C27="",D27="",E27="",G27="",H27="",I27=""),"Donnée manquante",((E27*60+F27)/(G27*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K27" s="22" t="str">
+        <f aca="false">IF(OR(J27="Donnée manquante",J27=""),"",$D$64-SUM($J$25:J27,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1176,15 +1165,14 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="21" t="str">
-        <f aca="false">IF(AND(B28="",C28="",D28="",E28="",G28="",I28="",J28=""),"",(IF(OR(B28="",C28="",D28="",E28="",G28="",I28="",J28=""),"Donnée manquante",((E28*60+F28)/(G28*60+H28)))))</f>
-        <v/>
-      </c>
-      <c r="L28" s="22" t="str">
-        <f aca="false">IF(OR(K28="Donnée manquante",K28=""),"",$D$64-SUM($K$25:K28,$C$49))</f>
+      <c r="H28" s="20"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="21" t="str">
+        <f aca="false">IF(AND(B28="",C28="",D28="",E28="",G28="",H28="",I28=""),"",(IF(OR(B28="",C28="",D28="",E28="",G28="",H28="",I28=""),"Donnée manquante",((E28*60+F28)/(G28*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K28" s="22" t="str">
+        <f aca="false">IF(OR(J28="Donnée manquante",J28=""),"",$D$64-SUM($J$25:J28,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1199,15 +1187,14 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="21" t="str">
-        <f aca="false">IF(AND(B29="",C29="",D29="",E29="",G29="",I29="",J29=""),"",(IF(OR(B29="",C29="",D29="",E29="",G29="",I29="",J29=""),"Donnée manquante",((E29*60+F29)/(G29*60+H29)))))</f>
-        <v/>
-      </c>
-      <c r="L29" s="22" t="str">
-        <f aca="false">IF(OR(K29="Donnée manquante",K29=""),"",$D$64-SUM($K$25:K29,$C$49))</f>
+      <c r="H29" s="20"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="21" t="str">
+        <f aca="false">IF(AND(B29="",C29="",D29="",E29="",G29="",H29="",I29=""),"",(IF(OR(B29="",C29="",D29="",E29="",G29="",H29="",I29=""),"Donnée manquante",((E29*60+F29)/(G29*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K29" s="22" t="str">
+        <f aca="false">IF(OR(J29="Donnée manquante",J29=""),"",$D$64-SUM($J$25:J29,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1222,15 +1209,14 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="21" t="str">
-        <f aca="false">IF(AND(B30="",C30="",D30="",E30="",G30="",I30="",J30=""),"",(IF(OR(B30="",C30="",D30="",E30="",G30="",I30="",J30=""),"Donnée manquante",((E30*60+F30)/(G30*60+H30)))))</f>
-        <v/>
-      </c>
-      <c r="L30" s="22" t="str">
-        <f aca="false">IF(OR(K30="Donnée manquante",K30=""),"",$D$64-SUM($K$25:K30,$C$49))</f>
+      <c r="H30" s="20"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="21" t="str">
+        <f aca="false">IF(AND(B30="",C30="",D30="",E30="",G30="",H30="",I30=""),"",(IF(OR(B30="",C30="",D30="",E30="",G30="",H30="",I30=""),"Donnée manquante",((E30*60+F30)/(G30*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K30" s="22" t="str">
+        <f aca="false">IF(OR(J30="Donnée manquante",J30=""),"",$D$64-SUM($J$25:J30,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1245,15 +1231,14 @@
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="21" t="str">
-        <f aca="false">IF(AND(B31="",C31="",D31="",E31="",G31="",I31="",J31=""),"",(IF(OR(B31="",C31="",D31="",E31="",G31="",I31="",J31=""),"Donnée manquante",((E31*60+F31)/(G31*60+H31)))))</f>
-        <v/>
-      </c>
-      <c r="L31" s="22" t="str">
-        <f aca="false">IF(OR(K31="Donnée manquante",K31=""),"",$D$64-SUM($K$25:K31,$C$49))</f>
+      <c r="H31" s="20"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="21" t="str">
+        <f aca="false">IF(AND(B31="",C31="",D31="",E31="",G31="",H31="",I31=""),"",(IF(OR(B31="",C31="",D31="",E31="",G31="",H31="",I31=""),"Donnée manquante",((E31*60+F31)/(G31*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K31" s="22" t="str">
+        <f aca="false">IF(OR(J31="Donnée manquante",J31=""),"",$D$64-SUM($J$25:J31,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1268,15 +1253,14 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="21" t="str">
-        <f aca="false">IF(AND(B32="",C32="",D32="",E32="",G32="",I32="",J32=""),"",(IF(OR(B32="",C32="",D32="",E32="",G32="",I32="",J32=""),"Donnée manquante",((E32*60+F32)/(G32*60+H32)))))</f>
-        <v/>
-      </c>
-      <c r="L32" s="22" t="str">
-        <f aca="false">IF(OR(K32="Donnée manquante",K32=""),"",$D$64-SUM($K$25:K32,$C$49))</f>
+      <c r="H32" s="20"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="21" t="str">
+        <f aca="false">IF(AND(B32="",C32="",D32="",E32="",G32="",H32="",I32=""),"",(IF(OR(B32="",C32="",D32="",E32="",G32="",H32="",I32=""),"Donnée manquante",((E32*60+F32)/(G32*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K32" s="22" t="str">
+        <f aca="false">IF(OR(J32="Donnée manquante",J32=""),"",$D$64-SUM($J$25:J32,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1291,15 +1275,14 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="21" t="str">
-        <f aca="false">IF(AND(B33="",C33="",D33="",E33="",G33="",I33="",J33=""),"",(IF(OR(B33="",C33="",D33="",E33="",G33="",I33="",J33=""),"Donnée manquante",((E33*60+F33)/(G33*60+H33)))))</f>
-        <v/>
-      </c>
-      <c r="L33" s="22" t="str">
-        <f aca="false">IF(OR(K33="Donnée manquante",K33=""),"",$D$64-SUM($K$25:K33,$C$49))</f>
+      <c r="H33" s="20"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="21" t="str">
+        <f aca="false">IF(AND(B33="",C33="",D33="",E33="",G33="",H33="",I33=""),"",(IF(OR(B33="",C33="",D33="",E33="",G33="",H33="",I33=""),"Donnée manquante",((E33*60+F33)/(G33*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K33" s="22" t="str">
+        <f aca="false">IF(OR(J33="Donnée manquante",J33=""),"",$D$64-SUM($J$25:J33,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1314,15 +1297,14 @@
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="21" t="str">
-        <f aca="false">IF(AND(B34="",C34="",D34="",E34="",G34="",I34="",J34=""),"",(IF(OR(B34="",C34="",D34="",E34="",G34="",I34="",J34=""),"Donnée manquante",((E34*60+F34)/(G34*60+H34)))))</f>
-        <v/>
-      </c>
-      <c r="L34" s="22" t="str">
-        <f aca="false">IF(OR(K34="Donnée manquante",K34=""),"",$D$64-SUM($K$25:K34,$C$49))</f>
+      <c r="H34" s="20"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="21" t="str">
+        <f aca="false">IF(AND(B34="",C34="",D34="",E34="",G34="",H34="",I34=""),"",(IF(OR(B34="",C34="",D34="",E34="",G34="",H34="",I34=""),"Donnée manquante",((E34*60+F34)/(G34*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K34" s="22" t="str">
+        <f aca="false">IF(OR(J34="Donnée manquante",J34=""),"",$D$64-SUM($J$25:J34,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1337,15 +1319,14 @@
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="21" t="str">
-        <f aca="false">IF(AND(B35="",C35="",D35="",E35="",G35="",I35="",J35=""),"",(IF(OR(B35="",C35="",D35="",E35="",G35="",I35="",J35=""),"Donnée manquante",((E35*60+F35)/(G35*60+H35)))))</f>
-        <v/>
-      </c>
-      <c r="L35" s="22" t="str">
-        <f aca="false">IF(OR(K35="Donnée manquante",K35=""),"",$D$64-SUM($K$25:K35,$C$49))</f>
+      <c r="H35" s="20"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="21" t="str">
+        <f aca="false">IF(AND(B35="",C35="",D35="",E35="",G35="",H35="",I35=""),"",(IF(OR(B35="",C35="",D35="",E35="",G35="",H35="",I35=""),"Donnée manquante",((E35*60+F35)/(G35*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K35" s="22" t="str">
+        <f aca="false">IF(OR(J35="Donnée manquante",J35=""),"",$D$64-SUM($J$25:J35,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1360,15 +1341,14 @@
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="21" t="str">
-        <f aca="false">IF(AND(B36="",C36="",D36="",E36="",G36="",I36="",J36=""),"",(IF(OR(B36="",C36="",D36="",E36="",G36="",I36="",J36=""),"Donnée manquante",((E36*60+F36)/(G36*60+H36)))))</f>
-        <v/>
-      </c>
-      <c r="L36" s="22" t="str">
-        <f aca="false">IF(OR(K36="Donnée manquante",K36=""),"",$D$64-SUM($K$25:K36,$C$49))</f>
+      <c r="H36" s="20"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="21" t="str">
+        <f aca="false">IF(AND(B36="",C36="",D36="",E36="",G36="",H36="",I36=""),"",(IF(OR(B36="",C36="",D36="",E36="",G36="",H36="",I36=""),"Donnée manquante",((E36*60+F36)/(G36*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K36" s="22" t="str">
+        <f aca="false">IF(OR(J36="Donnée manquante",J36=""),"",$D$64-SUM($J$25:J36,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1383,15 +1363,14 @@
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="21" t="str">
-        <f aca="false">IF(AND(B37="",C37="",D37="",E37="",G37="",I37="",J37=""),"",(IF(OR(B37="",C37="",D37="",E37="",G37="",I37="",J37=""),"Donnée manquante",((E37*60+F37)/(G37*60+H37)))))</f>
-        <v/>
-      </c>
-      <c r="L37" s="22" t="str">
-        <f aca="false">IF(OR(K37="Donnée manquante",K37=""),"",$D$64-SUM($K$25:K37,$C$49))</f>
+      <c r="H37" s="20"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="21" t="str">
+        <f aca="false">IF(AND(B37="",C37="",D37="",E37="",G37="",H37="",I37=""),"",(IF(OR(B37="",C37="",D37="",E37="",G37="",H37="",I37=""),"Donnée manquante",((E37*60+F37)/(G37*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K37" s="22" t="str">
+        <f aca="false">IF(OR(J37="Donnée manquante",J37=""),"",$D$64-SUM($J$25:J37,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1406,15 +1385,14 @@
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="21" t="str">
-        <f aca="false">IF(AND(B38="",C38="",D38="",E38="",G38="",I38="",J38=""),"",(IF(OR(B38="",C38="",D38="",E38="",G38="",I38="",J38=""),"Donnée manquante",((E38*60+F38)/(G38*60+H38)))))</f>
-        <v/>
-      </c>
-      <c r="L38" s="22" t="str">
-        <f aca="false">IF(OR(K38="Donnée manquante",K38=""),"",$D$64-SUM($K$25:K38,$C$49))</f>
+      <c r="H38" s="20"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="21" t="str">
+        <f aca="false">IF(AND(B38="",C38="",D38="",E38="",G38="",H38="",I38=""),"",(IF(OR(B38="",C38="",D38="",E38="",G38="",H38="",I38=""),"Donnée manquante",((E38*60+F38)/(G38*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K38" s="22" t="str">
+        <f aca="false">IF(OR(J38="Donnée manquante",J38=""),"",$D$64-SUM($J$25:J38,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1429,15 +1407,14 @@
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="21" t="str">
-        <f aca="false">IF(AND(B39="",C39="",D39="",E39="",G39="",I39="",J39=""),"",(IF(OR(B39="",C39="",D39="",E39="",G39="",I39="",J39=""),"Donnée manquante",((E39*60+F39)/(G39*60+H39)))))</f>
-        <v/>
-      </c>
-      <c r="L39" s="22" t="str">
-        <f aca="false">IF(OR(K39="Donnée manquante",K39=""),"",$D$64-SUM($K$25:K39,$C$49))</f>
+      <c r="H39" s="20"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="21" t="str">
+        <f aca="false">IF(AND(B39="",C39="",D39="",E39="",G39="",H39="",I39=""),"",(IF(OR(B39="",C39="",D39="",E39="",G39="",H39="",I39=""),"Donnée manquante",((E39*60+F39)/(G39*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K39" s="22" t="str">
+        <f aca="false">IF(OR(J39="Donnée manquante",J39=""),"",$D$64-SUM($J$25:J39,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1452,15 +1429,14 @@
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="21" t="str">
-        <f aca="false">IF(AND(B40="",C40="",D40="",E40="",G40="",I40="",J40=""),"",(IF(OR(B40="",C40="",D40="",E40="",G40="",I40="",J40=""),"Donnée manquante",((E40*60+F40)/(G40*60+H40)))))</f>
-        <v/>
-      </c>
-      <c r="L40" s="22" t="str">
-        <f aca="false">IF(OR(K40="Donnée manquante",K40=""),"",$D$64-SUM($K$25:K40,$C$49))</f>
+      <c r="H40" s="20"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="21" t="str">
+        <f aca="false">IF(AND(B40="",C40="",D40="",E40="",G40="",H40="",I40=""),"",(IF(OR(B40="",C40="",D40="",E40="",G40="",H40="",I40=""),"Donnée manquante",((E40*60+F40)/(G40*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K40" s="22" t="str">
+        <f aca="false">IF(OR(J40="Donnée manquante",J40=""),"",$D$64-SUM($J$25:J40,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1475,15 +1451,14 @@
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="21" t="str">
-        <f aca="false">IF(AND(B41="",C41="",D41="",E41="",G41="",I41="",J41=""),"",(IF(OR(B41="",C41="",D41="",E41="",G41="",I41="",J41=""),"Donnée manquante",((E41*60+F41)/(G41*60+H41)))))</f>
-        <v/>
-      </c>
-      <c r="L41" s="22" t="str">
-        <f aca="false">IF(OR(K41="Donnée manquante",K41=""),"",$D$64-SUM($K$25:K41,$C$49))</f>
+      <c r="H41" s="20"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="21" t="str">
+        <f aca="false">IF(AND(B41="",C41="",D41="",E41="",G41="",H41="",I41=""),"",(IF(OR(B41="",C41="",D41="",E41="",G41="",H41="",I41=""),"Donnée manquante",((E41*60+F41)/(G41*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K41" s="22" t="str">
+        <f aca="false">IF(OR(J41="Donnée manquante",J41=""),"",$D$64-SUM($J$25:J41,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1498,15 +1473,14 @@
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="21" t="str">
-        <f aca="false">IF(AND(B42="",C42="",D42="",E42="",G42="",I42="",J42=""),"",(IF(OR(B42="",C42="",D42="",E42="",G42="",I42="",J42=""),"Donnée manquante",((E42*60+F42)/(G42*60+H42)))))</f>
-        <v/>
-      </c>
-      <c r="L42" s="22" t="str">
-        <f aca="false">IF(OR(K42="Donnée manquante",K42=""),"",$D$64-SUM($K$25:K42,$C$49))</f>
+      <c r="H42" s="20"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="21" t="str">
+        <f aca="false">IF(AND(B42="",C42="",D42="",E42="",G42="",H42="",I42=""),"",(IF(OR(B42="",C42="",D42="",E42="",G42="",H42="",I42=""),"Donnée manquante",((E42*60+F42)/(G42*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K42" s="22" t="str">
+        <f aca="false">IF(OR(J42="Donnée manquante",J42=""),"",$D$64-SUM($J$25:J42,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1521,15 +1495,14 @@
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="21" t="str">
-        <f aca="false">IF(AND(B43="",C43="",D43="",E43="",G43="",I43="",J43=""),"",(IF(OR(B43="",C43="",D43="",E43="",G43="",I43="",J43=""),"Donnée manquante",((E43*60+F43)/(G43*60+H43)))))</f>
-        <v/>
-      </c>
-      <c r="L43" s="22" t="str">
-        <f aca="false">IF(OR(K43="Donnée manquante",K43=""),"",$D$64-SUM($K$25:K43,$C$49))</f>
+      <c r="H43" s="20"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="21" t="str">
+        <f aca="false">IF(AND(B43="",C43="",D43="",E43="",G43="",H43="",I43=""),"",(IF(OR(B43="",C43="",D43="",E43="",G43="",H43="",I43=""),"Donnée manquante",((E43*60+F43)/(G43*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K43" s="22" t="str">
+        <f aca="false">IF(OR(J43="Donnée manquante",J43=""),"",$D$64-SUM($J$25:J43,$C$49))</f>
         <v/>
       </c>
     </row>
@@ -1544,21 +1517,20 @@
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="26" t="str">
-        <f aca="false">IF(AND(B44="",C44="",D44="",E44="",G44="",I44="",J44=""),"",(IF(OR(B44="",C44="",D44="",E44="",G44="",I44="",J44=""),"Donnée manquante",((E44*60+F44)/(G44*60+H44)))))</f>
-        <v/>
-      </c>
-      <c r="L44" s="27" t="str">
-        <f aca="false">IF(OR(K44="Donnée manquante",K44=""),"",$D$64-SUM($K$25:K44,$C$49))</f>
+      <c r="H44" s="25"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="26" t="str">
+        <f aca="false">IF(AND(B44="",C44="",D44="",E44="",G44="",H44="",I44=""),"",(IF(OR(B44="",C44="",D44="",E44="",G44="",H44="",I44=""),"Donnée manquante",((E44*60+F44)/(G44*60+#REF!)))))</f>
+        <v/>
+      </c>
+      <c r="K44" s="27" t="str">
+        <f aca="false">IF(OR(J44="Donnée manquante",J44=""),"",$D$64-SUM($J$25:J44,$C$49))</f>
         <v/>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D46" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
@@ -1569,7 +1541,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -1583,13 +1555,13 @@
     </row>
     <row r="48" customFormat="false" ht="52.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="C48" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>32</v>
       </c>
       <c r="D48" s="28"/>
       <c r="E48" s="28"/>
@@ -1612,7 +1584,7 @@
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="29"/>
@@ -1620,7 +1592,7 @@
       <c r="E51" s="29"/>
       <c r="F51" s="29"/>
       <c r="G51" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
@@ -1629,12 +1601,12 @@
     </row>
     <row r="52" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
       <c r="D52" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
@@ -1646,18 +1618,18 @@
     </row>
     <row r="53" customFormat="false" ht="47.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" s="34"/>
       <c r="C53" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D53" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>39</v>
       </c>
       <c r="E53" s="34"/>
       <c r="F53" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
@@ -1719,7 +1691,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="29"/>
@@ -1729,7 +1701,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59" s="40"/>
       <c r="C59" s="41" t="n">
@@ -1737,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E59" s="40"/>
       <c r="F59" s="41" t="n">
@@ -1747,7 +1719,7 @@
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B61" s="42"/>
       <c r="C61" s="42"/>
@@ -1762,42 +1734,42 @@
         <v>16</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15"/>
       <c r="E62" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F62" s="15"/>
       <c r="G62" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H62" s="16"/>
     </row>
     <row r="63" customFormat="false" ht="47.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="43"/>
       <c r="B63" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="15" t="s">
+      <c r="E63" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="F63" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="F63" s="15" t="s">
-        <v>51</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" s="45" t="n">
         <v>0.567</v>
@@ -1811,7 +1783,7 @@
         <v>0.567</v>
       </c>
       <c r="E64" s="45" t="n">
-        <f aca="false">SUM(K25:K44)</f>
+        <f aca="false">SUM(J25:J44)</f>
         <v>0</v>
       </c>
       <c r="F64" s="45" t="n">
@@ -1839,23 +1811,13 @@
     <row r="67" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I67" s="1"/>
     </row>
-    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="A4:G19"/>
     <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A23:K23"/>
     <mergeCell ref="D46:J48"/>
     <mergeCell ref="A47:C47"/>
     <mergeCell ref="A51:F51"/>
@@ -1883,17 +1845,13 @@
     <mergeCell ref="G64:H64"/>
     <mergeCell ref="I64:K64"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation allowBlank="false" error="Un code corps comprend trois chiffres." errorStyle="stop" errorTitle="Mauvais code corps" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I25:I44" type="custom">
-      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(I25,"[0-9]{3}"))</formula1>
+  <dataValidations count="11">
+    <dataValidation allowBlank="false" error="Un code corps comprend trois chiffres." errorStyle="stop" errorTitle="Mauvais code corps" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H25:H44" type="custom">
+      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(H25,"[0-9]{3}"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Insérez entre 0 et 59 minutes." errorStyle="stop" errorTitle="Minute !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F25:F44" type="custom">
       <formula1>AND(F25&gt;=0,F25&lt;60)</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" error="Insérez des minutes, entre 0 et 59." errorStyle="stop" errorTitle="Minute !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H25:H44" type="custom">
-      <formula1>AND(H25&gt;=0,H25&lt;60)</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="L'ORS hebdomadaire la plus petite est 15 heures pour les enseignant-es.&#10;Pour les autres agent-es, l'ORS est de 1607 heures, temps partiel ou pas." errorStyle="stop" errorTitle="ORS" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G25:G44" type="custom">
@@ -1928,8 +1886,8 @@
       <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(A54,"^[A-Z].* \(.*\)$"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Exemple de RNE : 1234567G" errorStyle="stop" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J25:J44" type="custom">
-      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(J25,"^[0-9]{7}[A-Z]$"))</formula1>
+    <dataValidation allowBlank="false" error="Exemple de RNE : 1234567G" errorStyle="stop" errorTitle="Saisissez un RNE" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I25:I44" type="custom">
+      <formula1>ISTEXT(_xlfn.ORG.LIBREOFFICE.REGEX(I25,"^[0-9]{7}[A-Z]$"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Erreur de formule validité M./Mme
</commit_message>
<xml_diff>
--- a/template2021-2022.xlsx
+++ b/template2021-2022.xlsx
@@ -188,12 +188,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.########"/>
+    <numFmt numFmtId="168" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.########"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -450,7 +451,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,6 +544,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
@@ -575,7 +580,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -725,11 +730,11 @@
   </sheetPr>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.42"/>
@@ -1109,6 +1114,7 @@
         <f aca="false">IF(OR(J25="Donnée manquante",J25=""),"",$D$64-SUM($J$25:J25,$C$49))</f>
         <v/>
       </c>
+      <c r="L25" s="23"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="18" t="str">
@@ -1507,51 +1513,51 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="23" t="str">
+      <c r="A44" s="24" t="str">
         <f aca="false">$A$64</f>
         <v>Ain (01)</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="26" t="str">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="27" t="str">
         <f aca="false">IF(AND(B44="",C44="",D44="",E44="",G44="",H44="",I44=""),"",(IF(OR(B44="",C44="",D44="",E44="",G44="",H44="",I44=""),"Donnée manquante",((E44*60+F44)/(G44*60)))))</f>
         <v/>
       </c>
-      <c r="K44" s="27" t="str">
+      <c r="K44" s="28" t="str">
         <f aca="false">IF(OR(J44="Donnée manquante",J44=""),"",$D$64-SUM($J$25:J44,$C$49))</f>
         <v/>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D46" s="28" t="s">
+      <c r="D46" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="52.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="s">
@@ -1563,174 +1569,174 @@
       <c r="C48" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
     </row>
     <row r="49" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="30"/>
-      <c r="B49" s="26" t="n">
+      <c r="A49" s="31"/>
+      <c r="B49" s="27" t="n">
         <f aca="false">C49*1607/7</f>
         <v>0</v>
       </c>
-      <c r="C49" s="31" t="n">
+      <c r="C49" s="32" t="n">
         <f aca="false">A49*3.5/1607</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="32" t="s">
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="30"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="H51" s="32"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
     </row>
     <row r="52" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="33" t="s">
+      <c r="A52" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33" t="s">
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
     </row>
     <row r="53" customFormat="false" ht="47.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="34"/>
-      <c r="C53" s="35" t="s">
+      <c r="B53" s="35"/>
+      <c r="C53" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E53" s="34"/>
-      <c r="F53" s="35" t="s">
+      <c r="E53" s="35"/>
+      <c r="F53" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
-      <c r="I53" s="32"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
     </row>
     <row r="54" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
-      <c r="I54" s="32"/>
-      <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
     </row>
     <row r="55" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
     </row>
     <row r="56" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
     </row>
     <row r="57" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
+      <c r="A57" s="39"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
     </row>
     <row r="58" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="30"/>
     </row>
     <row r="59" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="41" t="n">
+      <c r="B59" s="41"/>
+      <c r="C59" s="42" t="n">
         <f aca="false">SUM(C54:C57)</f>
         <v>0</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="D59" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="E59" s="40"/>
-      <c r="F59" s="41" t="n">
+      <c r="E59" s="41"/>
+      <c r="F59" s="42" t="n">
         <f aca="false">SUM(F54:F57)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="42" t="s">
+      <c r="A61" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="43"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="43"/>
     </row>
     <row r="62" customFormat="false" ht="14.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="43" t="s">
+      <c r="A62" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B62" s="15" t="s">
@@ -1748,7 +1754,7 @@
       <c r="H62" s="16"/>
     </row>
     <row r="63" customFormat="false" ht="47.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="43"/>
+      <c r="A63" s="44"/>
       <c r="B63" s="15" t="s">
         <v>47</v>
       </c>
@@ -1768,39 +1774,39 @@
       <c r="H63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="45" t="n">
+      <c r="B64" s="46" t="n">
         <v>0.567</v>
       </c>
-      <c r="C64" s="45" t="n">
+      <c r="C64" s="46" t="n">
         <f aca="false">F59-C59</f>
         <v>0</v>
       </c>
-      <c r="D64" s="45" t="n">
+      <c r="D64" s="46" t="n">
         <f aca="false">B64+C64</f>
         <v>0.567</v>
       </c>
-      <c r="E64" s="45" t="n">
+      <c r="E64" s="46" t="n">
         <f aca="false">SUM(J25:J44)</f>
         <v>0</v>
       </c>
-      <c r="F64" s="45" t="n">
+      <c r="F64" s="46" t="n">
         <f aca="false">C49</f>
         <v>0</v>
       </c>
-      <c r="G64" s="46" t="str">
+      <c r="G64" s="47" t="str">
         <f aca="false">IF(SUM(E64:F64)&gt;D64,"Vous dépassez de "&amp;ROUND((SUM(E64:F64)-D64),3)&amp;" ETP",IF(SUM(E64:F64)&lt;=D64,"Vous rendez "&amp;ABS(ROUND(SUM(E64:F64)-D64,3))&amp;" ETP","Erreur"))</f>
         <v>Vous rendez 0,567 ETP</v>
       </c>
-      <c r="H64" s="46"/>
-      <c r="I64" s="47" t="str">
+      <c r="H64" s="47"/>
+      <c r="I64" s="48" t="str">
         <f aca="false">IF(E64+F64&gt;D64,"Trop d’ETP consommés : votre tableau sera refusé","Règles fédérales respectées")</f>
         <v>Règles fédérales respectées</v>
       </c>
-      <c r="J64" s="47"/>
-      <c r="K64" s="47"/>
+      <c r="J64" s="48"/>
+      <c r="K64" s="48"/>
     </row>
     <row r="65" customFormat="false" ht="13.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="17"/>
@@ -1887,7 +1893,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="C'est “M.” ou “Mme”. &#10;Pas d'espace dans tous les sens, pas d’abbréviation bizarre." errorStyle="stop" errorTitle="M. ou Mme" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B25:B44" type="custom">
-      <formula1>IF(B25=or("M.","Mme"),TRUE())</formula1>
+      <formula1>IF(OR(B25="M.",B25="Mme"),TRUE())</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>